<commit_message>
Fixed error in excel example
</commit_message>
<xml_diff>
--- a/exemple-valide.xlsx
+++ b/exemple-valide.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mario/Dropbox/Etalab/schema-hautes-remunerations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B97268C9-4DA1-934E-BB64-1AC0604F6F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D38DECBE-4BD2-444D-A6A5-277EF9520C96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{68327E07-F75B-954C-AA76-F17C759F1937}"/>
+    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15540" xr2:uid="{0B3458AC-58AA-D34F-A842-1D3036549786}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="exemple_valide" localSheetId="0">Feuil1!$A$1:$H$3</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,27 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{FC919531-DD2A-544F-997B-06BE5325C282}" name="exemple-valide" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="/Users/mario/Dropbox/Etalab/schema-hautes-remunerations/exemple-valide.csv" decimal="," thousands=" " tab="0" semicolon="1">
-      <textFields count="8">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>siren</t>
   </si>
@@ -79,9 +57,6 @@
   </si>
   <si>
     <t>commentaires</t>
-  </si>
-  <si>
-    <t>110 043 015</t>
   </si>
   <si>
     <t>Ministère de l'éducation nationale et de la jeunesse et  ministère de l'enseignement supérieur, de la recherche et de l'innovation</t>
@@ -137,10 +112,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="exemple-valide" connectionId="1" xr16:uid="{1611F40C-B750-A74A-A984-A025EAFBC2DF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,22 +410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9830E688-58EA-0344-992A-3259DD6E954C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68012222-CB58-F849-BE33-FBCC38C99F22}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -483,11 +446,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>110043015</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2">
         <v>2018</v>
@@ -506,11 +469,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>110043015</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3">
         <v>2019</v>

</xml_diff>